<commit_message>
Added new drill guide and partslist
</commit_message>
<xml_diff>
--- a/BigMuffPi-Partlists_versions.xlsx
+++ b/BigMuffPi-Partlists_versions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="120">
   <si>
     <t>Big Muff Pi Versions</t>
   </si>
@@ -296,9 +296,6 @@
     <t>1uF Film/Elc</t>
   </si>
   <si>
-    <t>Violet Rams</t>
-  </si>
-  <si>
     <t>100ohm</t>
   </si>
   <si>
@@ -375,6 +372,21 @@
   </si>
   <si>
     <t>Xenocoder Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GGG Violet Rams 2 </t>
+  </si>
+  <si>
+    <t>Violet Ram's 1</t>
+  </si>
+  <si>
+    <t>33k</t>
+  </si>
+  <si>
+    <t>560ohm</t>
+  </si>
+  <si>
+    <t>430pF Cer</t>
   </si>
 </sst>
 </file>
@@ -522,8 +534,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -546,11 +568,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -829,25 +861,26 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J55"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>28</v>
       </c>
@@ -855,28 +888,31 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -887,7 +923,7 @@
         <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>41</v>
@@ -901,14 +937,17 @@
       <c r="H3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -933,14 +972,17 @@
       <c r="H4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -965,14 +1007,17 @@
       <c r="H5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -983,28 +1028,31 @@
         <v>83</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1015,13 +1063,13 @@
         <v>84</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>39</v>
@@ -1029,14 +1077,17 @@
       <c r="H7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1047,7 +1098,7 @@
         <v>67</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>67</v>
@@ -1061,14 +1112,17 @@
       <c r="H8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="J8" s="11" t="s">
+      <c r="I8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1079,7 +1133,7 @@
         <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>37</v>
@@ -1093,14 +1147,17 @@
       <c r="H9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1116,8 +1173,8 @@
       <c r="E10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>84</v>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>84</v>
@@ -1125,14 +1182,17 @@
       <c r="H10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1157,14 +1217,17 @@
       <c r="H11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1189,46 +1252,52 @@
       <c r="H12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="K12" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="J13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="K13" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1239,28 +1308,31 @@
         <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="J14" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K14" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1276,8 +1348,8 @@
       <c r="E15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>84</v>
+      <c r="F15" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>84</v>
@@ -1285,14 +1357,17 @@
       <c r="H15" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="K15" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1317,14 +1392,17 @@
       <c r="H16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="K16" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1349,14 +1427,17 @@
       <c r="H17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="K17" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1367,28 +1448,31 @@
         <v>40</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>97</v>
+        <v>89</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="J18" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="K18" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1399,13 +1483,13 @@
         <v>85</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>39</v>
+      <c r="F19" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>39</v>
@@ -1413,14 +1497,17 @@
       <c r="H19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="K19" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1430,14 +1517,14 @@
       <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>36</v>
+      <c r="F20" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>36</v>
@@ -1445,14 +1532,17 @@
       <c r="H20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1463,28 +1553,31 @@
         <v>41</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>98</v>
+      <c r="F21" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="J21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="K21" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1495,7 +1588,7 @@
         <v>68</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>68</v>
@@ -1509,14 +1602,17 @@
       <c r="H22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="J22" s="11" t="s">
+      <c r="I22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="K22" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1541,14 +1637,17 @@
       <c r="H23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I23" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="J23" s="11" t="s">
+      <c r="I23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K23" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1558,14 +1657,14 @@
       <c r="C24" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>34</v>
+      <c r="D24" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>82</v>
+      <c r="F24" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>82</v>
@@ -1573,14 +1672,17 @@
       <c r="H24" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J24" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="K24" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1593,26 +1695,29 @@
       <c r="D25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="H25" s="1" t="s">
+      <c r="F25" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="H25" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="J25" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K25" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1622,8 +1727,8 @@
       <c r="C26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>84</v>
+      <c r="D26" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>84</v>
@@ -1637,14 +1742,17 @@
       <c r="H26" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J26" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="K26" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1655,7 +1763,7 @@
         <v>67</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>67</v>
@@ -1669,14 +1777,17 @@
       <c r="H27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1701,14 +1812,17 @@
       <c r="H28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="I28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J28" s="11" t="s">
+      <c r="J28" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K28" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1733,18 +1847,21 @@
       <c r="H29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I29" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="J29" s="11" t="s">
+      <c r="I29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="K29" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I30" s="10"/>
-      <c r="J30" s="11"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J30" s="10"/>
+      <c r="K30" s="11"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -1769,14 +1886,17 @@
       <c r="H31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I31" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J31" s="11" t="s">
+      <c r="I31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K31" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -1786,29 +1906,32 @@
       <c r="C32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F32" s="7" t="s">
+      <c r="D32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>91</v>
+      <c r="E32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="J32" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K32" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -1821,11 +1944,11 @@
       <c r="D33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>60</v>
+      <c r="E33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>60</v>
@@ -1833,14 +1956,17 @@
       <c r="H33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I33" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J33" s="11" t="s">
+      <c r="I33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -1853,11 +1979,11 @@
       <c r="D34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>60</v>
+      <c r="E34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>60</v>
@@ -1865,14 +1991,17 @@
       <c r="H34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I34" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J34" s="11" t="s">
+      <c r="I34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K34" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -1882,29 +2011,32 @@
       <c r="C35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>91</v>
+      <c r="E35" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="J35" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K35" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -1920,8 +2052,8 @@
       <c r="E36" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>62</v>
+      <c r="F36" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>62</v>
@@ -1929,14 +2061,17 @@
       <c r="H36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I36" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="J36" s="11" t="s">
+      <c r="I36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K36" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -1946,14 +2081,14 @@
       <c r="C37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>60</v>
+      <c r="D37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>60</v>
@@ -1961,14 +2096,17 @@
       <c r="H37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I37" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J37" s="11" t="s">
+      <c r="I37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K37" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -1978,29 +2116,32 @@
       <c r="C38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>91</v>
+      <c r="E38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="J38" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K38" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -2016,8 +2157,8 @@
       <c r="E39" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>62</v>
+      <c r="F39" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>62</v>
@@ -2025,14 +2166,17 @@
       <c r="H39" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I39" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="J39" s="11" t="s">
+      <c r="I39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K39" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2057,14 +2201,17 @@
       <c r="H40" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I40" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="J40" s="11" t="s">
+      <c r="I40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K40" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2089,14 +2236,17 @@
       <c r="H41" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I41" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="J41" s="11" t="s">
+      <c r="I41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="K41" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2121,14 +2271,17 @@
       <c r="H42" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I42" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J42" s="11" t="s">
+      <c r="I42" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K42" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -2153,22 +2306,25 @@
       <c r="H43" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I43" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J43" s="11" t="s">
+      <c r="I43" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K43" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>58</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>60</v>
+      <c r="C44" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>65</v>
@@ -2185,14 +2341,17 @@
       <c r="H44" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I44" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="J44" s="11" t="s">
+      <c r="I44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K44" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2217,18 +2376,21 @@
       <c r="H45" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I45" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="J45" s="11" t="s">
+      <c r="I45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="K45" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I46" s="10"/>
-      <c r="J46" s="11"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J46" s="10"/>
+      <c r="K46" s="11"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -2253,14 +2415,17 @@
       <c r="H47" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I47" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J47" s="11" t="s">
+      <c r="I47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K47" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -2285,14 +2450,17 @@
       <c r="H48" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I48" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J48" s="11" t="s">
+      <c r="I48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K48" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>71</v>
       </c>
@@ -2317,14 +2485,17 @@
       <c r="H49" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I49" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J49" s="11" t="s">
+      <c r="I49" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K49" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>72</v>
       </c>
@@ -2349,14 +2520,17 @@
       <c r="H50" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I50" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J50" s="11" t="s">
+      <c r="I50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K50" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>73</v>
       </c>
@@ -2381,12 +2555,15 @@
       <c r="H51" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I51" s="12" t="s">
+      <c r="I51" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J51" s="11"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J51" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K51" s="11"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -2405,20 +2582,23 @@
       <c r="F52" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>80</v>
+      <c r="G52" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I52" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="J52" s="11" t="s">
+      <c r="I52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="K52" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>77</v>
       </c>
@@ -2437,20 +2617,23 @@
       <c r="F53" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>80</v>
+      <c r="G53" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I53" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="J53" s="11" t="s">
+      <c r="I53" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="K53" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>78</v>
       </c>
@@ -2469,20 +2652,23 @@
       <c r="F54" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>80</v>
+      <c r="G54" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I54" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="J54" s="11" t="s">
+      <c r="I54" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="K54" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -2501,22 +2687,25 @@
       <c r="F55" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>80</v>
+      <c r="G55" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I55" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="J55" s="14" t="s">
+      <c r="I55" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J55" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="K55" s="14" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="71" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="64" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>